<commit_message>
update some oncho forms
</commit_message>
<xml_diff>
--- a/Dimagi/ESPEN Collect forms/oncho_2_river_inspection.xlsx
+++ b/Dimagi/ESPEN Collect forms/oncho_2_river_inspection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\Dimagi\ESPEN Collect forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E395E292-BC69-4CD3-A310-205F6B55BE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FCA5C1-4CBE-4326-BF91-09A866ED172E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="133">
   <si>
     <t>type</t>
   </si>
@@ -440,16 +440,22 @@
     <t>The PH must be between 0 and 14</t>
   </si>
   <si>
-    <t>oncho_2_river_inspection_v3</t>
-  </si>
-  <si>
-    <t>2. River inspection Form V3</t>
-  </si>
-  <si>
     <t>.&lt;=date(today())</t>
   </si>
   <si>
     <t>The date cannot be in the future</t>
+  </si>
+  <si>
+    <t>2. River inspection Form V4</t>
+  </si>
+  <si>
+    <t>oncho_2_river_inspection_v4</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>Enter the Community Name</t>
   </si>
 </sst>
 </file>
@@ -970,13 +976,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1095,7 +1101,7 @@
         <v>84</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
@@ -1114,10 +1120,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="7"/>
@@ -1137,14 +1143,14 @@
         <v>11</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="11"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="9"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -1155,15 +1161,15 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="7"/>
@@ -1178,24 +1184,20 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>130</v>
-      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
@@ -1207,18 +1209,22 @@
     </row>
     <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>128</v>
+      </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7" t="s">
@@ -1230,13 +1236,13 @@
     </row>
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="7"/>
@@ -1248,50 +1254,48 @@
         <v>9</v>
       </c>
       <c r="K10" s="7"/>
-      <c r="L10" s="12"/>
+      <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="L11" s="12"/>
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="9"/>
       <c r="H12" s="7" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7" t="s">
@@ -1301,25 +1305,23 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="H13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7" t="s">
         <v>9</v>
@@ -1328,20 +1330,24 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7" t="s">
@@ -1356,10 +1362,10 @@
         <v>35</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="7"/>
@@ -1374,23 +1380,21 @@
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="7" t="s">
-        <v>115</v>
-      </c>
+      <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="s">
         <v>9</v>
@@ -1399,21 +1403,23 @@
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
     </row>
-    <row r="17" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7" t="s">
         <v>9</v>
@@ -1424,21 +1430,19 @@
     </row>
     <row r="18" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="7" t="s">
-        <v>116</v>
-      </c>
+      <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7" t="s">
         <v>9</v>
@@ -1447,36 +1451,40 @@
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
     </row>
-    <row r="19" spans="1:13" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+      <c r="J19" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="7"/>
@@ -1494,10 +1502,10 @@
         <v>93</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="7"/>
@@ -1515,10 +1523,10 @@
         <v>93</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="7"/>
@@ -1531,58 +1539,64 @@
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
     </row>
-    <row r="23" spans="1:13" s="10" customFormat="1" ht="267.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>125</v>
-      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="10" customFormat="1" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="9"/>
+      <c r="F24" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
+      <c r="J24" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
+    <row r="25" spans="1:13" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>119</v>
+      </c>
       <c r="D25" s="9"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1594,16 +1608,10 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13" s="10" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>113</v>
-      </c>
+    <row r="26" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -1615,24 +1623,20 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="10" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>122</v>
-      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="9"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
@@ -1640,31 +1644,37 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
+        <v>123</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
       <c r="J28" s="7"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
     </row>
     <row r="29" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -1677,6 +1687,25 @@
       <c r="K29" s="14"/>
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
+    </row>
+    <row r="30" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1930,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1955,10 +1984,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
demo: add update forms
</commit_message>
<xml_diff>
--- a/Dimagi/ESPEN Collect forms/oncho_2_river_inspection.xlsx
+++ b/Dimagi/ESPEN Collect forms/oncho_2_river_inspection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\Dimagi\ESPEN Collect forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FCA5C1-4CBE-4326-BF91-09A866ED172E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8F2497-356F-4C20-A5ED-2AB870E37FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="134">
   <si>
     <t>type</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t xml:space="preserve">What are the characteristics of the river? Please choose as many as apply. </t>
-  </si>
-  <si>
-    <t>Select Site Name</t>
   </si>
   <si>
     <t>Insecurity</t>
@@ -446,16 +443,22 @@
     <t>The date cannot be in the future</t>
   </si>
   <si>
-    <t>2. River inspection Form V4</t>
-  </si>
-  <si>
-    <t>oncho_2_river_inspection_v4</t>
-  </si>
-  <si>
-    <t>site</t>
-  </si>
-  <si>
     <t>Enter the Community Name</t>
+  </si>
+  <si>
+    <t>oncho_2_river_inspection_v5</t>
+  </si>
+  <si>
+    <t>2. River inspection Form V5</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>r_State</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -978,11 +981,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1073,13 +1076,13 @@
     </row>
     <row r="3" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="7"/>
@@ -1091,6 +1094,7 @@
         <v>9</v>
       </c>
       <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1098,10 +1102,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="7"/>
@@ -1120,10 +1124,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>73</v>
+        <v>128</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="7"/>
@@ -1135,7 +1139,6 @@
         <v>9</v>
       </c>
       <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1220,10 +1223,10 @@
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>128</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -1282,7 +1285,7 @@
     </row>
     <row r="12" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>43</v>
@@ -1295,7 +1298,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="9"/>
       <c r="H12" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7" t="s">
@@ -1320,7 +1323,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="9"/>
       <c r="H13" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7" t="s">
@@ -1332,21 +1335,21 @@
     </row>
     <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -1405,7 +1408,7 @@
     </row>
     <row r="17" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>47</v>
@@ -1418,7 +1421,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="9"/>
       <c r="H17" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7" t="s">
@@ -1453,7 +1456,7 @@
     </row>
     <row r="19" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>49</v>
@@ -1466,7 +1469,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="9"/>
       <c r="H19" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7" t="s">
@@ -1478,7 +1481,7 @@
     </row>
     <row r="20" spans="1:13" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>50</v>
@@ -1499,7 +1502,7 @@
     </row>
     <row r="21" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>51</v>
@@ -1520,7 +1523,7 @@
     </row>
     <row r="22" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>52</v>
@@ -1541,7 +1544,7 @@
     </row>
     <row r="23" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>53</v>
@@ -1562,7 +1565,7 @@
     </row>
     <row r="24" spans="1:13" s="10" customFormat="1" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>54</v>
@@ -1573,10 +1576,10 @@
       <c r="D24" s="9"/>
       <c r="E24" s="7"/>
       <c r="F24" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -1595,7 +1598,7 @@
         <v>55</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="7"/>
@@ -1625,13 +1628,13 @@
     </row>
     <row r="27" spans="1:13" s="10" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="7"/>
@@ -1649,18 +1652,18 @@
         <v>35</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
@@ -1775,90 +1778,90 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1866,10 +1869,10 @@
         <v>54</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1877,10 +1880,10 @@
         <v>54</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1888,10 +1891,10 @@
         <v>54</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -1899,10 +1902,10 @@
         <v>54</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -1910,10 +1913,10 @@
         <v>54</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1921,10 +1924,10 @@
         <v>54</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1932,10 +1935,10 @@
         <v>54</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1943,10 +1946,10 @@
         <v>54</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1959,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1984,10 +1987,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>

</xml_diff>